<commit_message>
fine schematico parte 2
</commit_message>
<xml_diff>
--- a/Tesi/BOM_singola_scheda.xlsx
+++ b/Tesi/BOM_singola_scheda.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\desktop\Tesi-2021\Tesi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AD6D8CF-2EEB-4ACE-9DAE-AD2D42D48DDB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E70FA5-FFE8-4051-B8A2-078A66823AA9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1E76902F-CB79-4AAF-A61B-A07AC3A8CE70}"/>
+    <workbookView xWindow="0" yWindow="2052" windowWidth="17280" windowHeight="8964" xr2:uid="{1E76902F-CB79-4AAF-A61B-A07AC3A8CE70}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -632,7 +632,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -667,7 +667,7 @@
         <v>6</v>
       </c>
       <c r="D2" s="2">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.4">

</xml_diff>